<commit_message>
Updating LCFS factors for FF55 scenario
</commit_message>
<xml_diff>
--- a/InputData/trans/BPoEFUbVT/BAU Perc of Each Fuel Used by Veh Tech.xlsx
+++ b/InputData/trans/BPoEFUbVT/BAU Perc of Each Fuel Used by Veh Tech.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\trans\BPoEFUbVT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA6BD84-8198-4B20-B86C-AB22CB0E654A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAFA0349-7373-4E17-9282-A208647C419A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="975" windowWidth="16695" windowHeight="15135" tabRatio="920" firstSheet="82" activeTab="84" xr2:uid="{4149C2B6-5FC6-4025-B0A7-5DEF302FBE20}"/>
+    <workbookView xWindow="4545" yWindow="1875" windowWidth="23910" windowHeight="15135" tabRatio="920" firstSheet="4" activeTab="4" xr2:uid="{4149C2B6-5FC6-4025-B0A7-5DEF302FBE20}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="103" r:id="rId1"/>
@@ -1073,8 +1073,8 @@
     <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="11" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Body: normal cell" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4273,91 +4273,91 @@
       <c r="A4" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="93">
+      <c r="B4" s="92">
         <v>0.96209995764645662</v>
       </c>
-      <c r="C4" s="93">
+      <c r="C4" s="92">
         <v>0.96070004054939806</v>
       </c>
-      <c r="D4" s="93">
+      <c r="D4" s="92">
         <v>0.95939995161511238</v>
       </c>
-      <c r="E4" s="93">
+      <c r="E4" s="92">
         <v>0.95789986771473112</v>
       </c>
-      <c r="F4" s="93">
+      <c r="F4" s="92">
         <v>0.95630011616147381</v>
       </c>
-      <c r="G4" s="93">
+      <c r="G4" s="92">
         <v>0.95450014869517874</v>
       </c>
-      <c r="H4" s="93">
+      <c r="H4" s="92">
         <v>0.95259986397834218</v>
       </c>
-      <c r="I4" s="93">
+      <c r="I4" s="92">
         <v>0.95050001747082391</v>
       </c>
-      <c r="J4" s="93">
+      <c r="J4" s="92">
         <v>0.94820015364122834</v>
       </c>
-      <c r="K4" s="93">
+      <c r="K4" s="92">
         <v>0.94619984757693842</v>
       </c>
-      <c r="L4" s="93">
+      <c r="L4" s="92">
         <v>0.94399983883977989</v>
       </c>
-      <c r="M4" s="93">
+      <c r="M4" s="92">
         <v>0.94180012505900423</v>
       </c>
-      <c r="N4" s="93">
+      <c r="N4" s="92">
         <v>0.9393999215918265</v>
       </c>
-      <c r="O4" s="93">
+      <c r="O4" s="92">
         <v>0.93690015579991637</v>
       </c>
-      <c r="P4" s="93">
+      <c r="P4" s="92">
         <v>0.9342000944113068</v>
       </c>
-      <c r="Q4" s="93">
+      <c r="Q4" s="92">
         <v>0.93140006821652233</v>
       </c>
-      <c r="R4" s="93">
+      <c r="R4" s="92">
         <v>0.9285002029788626</v>
       </c>
-      <c r="S4" s="93">
+      <c r="S4" s="92">
         <v>0.92539985076973297</v>
       </c>
-      <c r="T4" s="93">
+      <c r="T4" s="92">
         <v>0.92219993424385949</v>
       </c>
-      <c r="U4" s="93">
+      <c r="U4" s="92">
         <v>0.91889977050488014</v>
       </c>
-      <c r="V4" s="93">
+      <c r="V4" s="92">
         <v>0.91530000601008632</v>
       </c>
-      <c r="W4" s="93">
+      <c r="W4" s="92">
         <v>0.91160001789315837</v>
       </c>
-      <c r="X4" s="93">
+      <c r="X4" s="92">
         <v>0.90769994239305962</v>
       </c>
-      <c r="Y4" s="93">
+      <c r="Y4" s="92">
         <v>0.90370001084346463</v>
       </c>
-      <c r="Z4" s="93">
+      <c r="Z4" s="92">
         <v>0.8995000555173126</v>
       </c>
-      <c r="AA4" s="93">
+      <c r="AA4" s="92">
         <v>0.89520001508440983</v>
       </c>
-      <c r="AB4" s="93">
+      <c r="AB4" s="92">
         <v>0.89080007602277711</v>
       </c>
-      <c r="AC4" s="93">
+      <c r="AC4" s="92">
         <v>0.88630014322802031</v>
       </c>
-      <c r="AD4" s="93">
+      <c r="AD4" s="92">
         <v>0.88180001191630419</v>
       </c>
       <c r="AE4" s="1">
@@ -59126,8 +59126,8 @@
   </sheetPr>
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59520,11 +59520,11 @@
       <c r="AD4" s="92">
         <v>0.93359990871754606</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AE4" s="93">
         <f>POTEnCIA!AY25/POTEnCIA!AY24</f>
         <v>0.9354597439318284</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AF4" s="93">
         <f>POTEnCIA!AZ25/POTEnCIA!AZ24</f>
         <v>0.93364239320421838</v>
       </c>
@@ -97588,7 +97588,7 @@
   </sheetPr>
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>

</xml_diff>